<commit_message>
Kleine Änderung am Projektplan
</commit_message>
<xml_diff>
--- a/Artefakte/ProjektplanV0.22.xlsx
+++ b/Artefakte/ProjektplanV0.22.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\6. Semester\EIS\EISSS19SchoenbergerTissen\Artefakte\1. Iteration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\6. Semester\EIS\EISSS19SchoenbergerTissen\Artefakte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9266DBB2-1F1D-4FF9-97D7-5BD7987787AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EE34D4-024D-4AE9-B5F8-4B87038D7E63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{49FFB486-0252-4090-A15B-F7AC9F70B8C0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t>EIS Projektplan von Malte Schönberger und Arthur Tissen</t>
   </si>
@@ -432,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -472,6 +472,8 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -788,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2061AD1A-F9E1-475E-99DF-2969214ACCAE}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -851,11 +853,11 @@
       <c r="F4" s="12"/>
       <c r="G4" s="20">
         <f>SUM(G5:G12)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H4" s="21">
         <f>SUM(H5:H12)</f>
-        <v>23</v>
+        <v>32.5</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>2</v>
@@ -871,10 +873,10 @@
       <c r="E5" s="11"/>
       <c r="F5" s="2"/>
       <c r="G5" s="24">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H5" s="25">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>3</v>
@@ -890,10 +892,10 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="22">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H6" s="23">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I6" s="26" t="s">
         <v>4</v>
@@ -943,10 +945,10 @@
       <c r="E9" s="11"/>
       <c r="F9" s="2"/>
       <c r="G9" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -959,10 +961,10 @@
       <c r="E10" s="9"/>
       <c r="F10" s="2"/>
       <c r="G10" s="22">
+        <v>3</v>
+      </c>
+      <c r="H10" s="23">
         <v>2</v>
-      </c>
-      <c r="H10" s="23">
-        <v>1.5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
@@ -1010,9 +1012,12 @@
       <c r="F13" s="12"/>
       <c r="G13" s="20">
         <f>SUM(G14:G21)</f>
-        <v>40</v>
-      </c>
-      <c r="H13" s="21"/>
+        <v>44</v>
+      </c>
+      <c r="H13" s="21">
+        <f>SUM(H14:H22)</f>
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="16"/>
@@ -1024,7 +1029,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="2"/>
       <c r="G14" s="22">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H14" s="23">
         <v>6</v>
@@ -1149,610 +1154,616 @@
       <c r="J21" s="33"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A22" s="15"/>
-      <c r="B22" s="13">
-        <v>3</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="20">
-        <f>SUM(G23:G24)</f>
-        <v>27</v>
-      </c>
-      <c r="H22" s="21"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39">
+        <v>8</v>
+      </c>
+      <c r="H22" s="39">
+        <v>8</v>
+      </c>
       <c r="I22" s="33"/>
       <c r="J22" s="33"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A23" s="16"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="13">
+        <v>3</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="20">
+        <f>SUM(G24:G25)</f>
+        <v>27</v>
+      </c>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="16"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="22">
+      <c r="E24" s="8"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="22">
         <v>12</v>
       </c>
-      <c r="H23" s="23"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A24" s="17"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10" t="s">
+      <c r="H24" s="23"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" s="17"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="24">
+      <c r="E25" s="10"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="24">
         <v>15</v>
       </c>
-      <c r="H24" s="25"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A25" s="15"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13" t="s">
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="15"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="20">
-        <f>SUM(G26:G30)</f>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="20">
+        <f>SUM(G27:G31)</f>
         <v>41</v>
       </c>
-      <c r="H25" s="21"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A26" s="17"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10" t="s">
+      <c r="H26" s="21"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="17"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="24">
+      <c r="E27" s="10"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="24">
         <v>10</v>
       </c>
-      <c r="H26" s="25"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A27" s="16"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8" t="s">
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" s="16"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="22">
+      <c r="E28" s="32"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="22">
         <v>8</v>
       </c>
-      <c r="H27" s="23"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A28" s="17"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10" t="s">
+      <c r="H28" s="23"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" s="17"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="24">
+      <c r="F29" s="2"/>
+      <c r="G29" s="24">
         <v>10</v>
       </c>
-      <c r="H28" s="25"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A29" s="16">
+      <c r="H29" s="25"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" s="16">
         <v>5</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="8" t="s">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="22">
+      <c r="F30" s="2"/>
+      <c r="G30" s="22">
         <v>12</v>
       </c>
-      <c r="H29" s="23"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27" t="s">
+      <c r="H30" s="23"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="27">
+      <c r="E31" s="27"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="40">
         <v>1</v>
       </c>
-      <c r="H30" s="27"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A31" s="32"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32" t="s">
+      <c r="H31" s="27"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A32" s="15"/>
-      <c r="B32" s="28">
+      <c r="E32" s="32"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="15"/>
+      <c r="B33" s="28">
         <v>4</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C33" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="21"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="21"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32" t="s">
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27" t="s">
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32" t="s">
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A37" s="32"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" s="27"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27" t="s">
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" s="27"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="32"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32" t="s">
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A39" s="32"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27" t="s">
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" s="32"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32" t="s">
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A41" s="32"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A41" s="27"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27" t="s">
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32" t="s">
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27" t="s">
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28">
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A45" s="28"/>
+      <c r="B45" s="28">
         <v>5</v>
       </c>
-      <c r="C44" s="28" t="s">
+      <c r="C45" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27" t="s">
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="32"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32" t="s">
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27" t="s">
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32" t="s">
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A49" s="32"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A49" s="27"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27" t="s">
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A50" s="37"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32" t="s">
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A51" s="37"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="E50" s="32"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A51" s="27"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27" t="s">
+      <c r="E51" s="32"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A52" s="35"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28" t="s">
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A53" s="35"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A53" s="27"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27" t="s">
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A54" s="32"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32" t="s">
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A55" s="32"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A55" s="27"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27" t="s">
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A56" s="37"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32" t="s">
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A57" s="37"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E56" s="32"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A57" s="27"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27" t="s">
+      <c r="E57" s="32"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A58" s="28"/>
-      <c r="B58" s="28">
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="27"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A59" s="28"/>
+      <c r="B59" s="28">
         <v>6</v>
       </c>
-      <c r="C58" s="28" t="s">
+      <c r="C59" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="28"/>
-      <c r="H58" s="28"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A59" s="27"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27" t="s">
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="28"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A60" s="32"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32" t="s">
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A61" s="32"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A61" s="27"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27" t="s">
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="32"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A62" s="32"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32" t="s">
+      <c r="E62" s="27"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="27"/>
+      <c r="H62" s="27"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A63" s="32"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A63" s="27"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27" t="s">
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A64" s="27"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="27"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A64" s="28"/>
-      <c r="B64" s="28"/>
-      <c r="C64" s="28" t="s">
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A65" s="28"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D64" s="28"/>
-      <c r="E64" s="28"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="28"/>
-      <c r="H64" s="28"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A65" s="27"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27" t="s">
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A66" s="27"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="27"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A66" s="32"/>
-      <c r="B66" s="32"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32" t="s">
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="27"/>
+      <c r="H66" s="27"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A67" s="32"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F66" s="32"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A67" s="27"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27" t="s">
+      <c r="F67" s="32"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="32"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A68" s="32"/>
-      <c r="B68" s="32"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="32" t="s">
+      <c r="F68" s="27"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A69" s="32"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E68" s="32"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="32"/>
-      <c r="H68" s="32"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A69" s="30"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
-      <c r="G69" s="30"/>
-      <c r="H69" s="30"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="32"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="30"/>

</xml_diff>